<commit_message>
payslip generate issue fixed
</commit_message>
<xml_diff>
--- a/ems_CoreService/ApplicationFiles/SampleExcel/HolidaySample.xlsx
+++ b/ems_CoreService/ApplicationFiles/SampleExcel/HolidaySample.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">CompanyId</t>
   </si>
   <si>
-    <t xml:space="preserve">StartDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EndDate</t>
+    <t xml:space="preserve">HolidayDate</t>
   </si>
   <si>
     <t xml:space="preserve">EventName</t>
@@ -79,7 +76,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -102,12 +99,6 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,7 +142,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,10 +160,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,21 +201,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AM2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:AM2"/>
-  <tableColumns count="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AL2" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:AL2"/>
+  <tableColumns count="38">
     <tableColumn id="1" name="CompanyId"/>
-    <tableColumn id="2" name="StartDate"/>
-    <tableColumn id="3" name="EndDate"/>
-    <tableColumn id="4" name="EventName"/>
-    <tableColumn id="5" name="IsHoliday"/>
-    <tableColumn id="6" name="IsHalfDay"/>
-    <tableColumn id="7" name="DescriptionNote"/>
-    <tableColumn id="8" name="ApplicableFor"/>
-    <tableColumn id="9" name="Year"/>
-    <tableColumn id="10" name="IsPublicHoliday"/>
-    <tableColumn id="11" name="IsCompanyCustomHoliday"/>
-    <tableColumn id="12" name="Country"/>
+    <tableColumn id="2" name="HolidayDate"/>
+    <tableColumn id="3" name="EventName"/>
+    <tableColumn id="4" name="IsHoliday"/>
+    <tableColumn id="5" name="IsHalfDay"/>
+    <tableColumn id="6" name="DescriptionNote"/>
+    <tableColumn id="7" name="ApplicableFor"/>
+    <tableColumn id="8" name="Year"/>
+    <tableColumn id="9" name="IsPublicHoliday"/>
+    <tableColumn id="10" name="IsCompanyCustomHoliday"/>
+    <tableColumn id="11" name="Country"/>
+    <tableColumn id="12" name=""/>
     <tableColumn id="13" name=""/>
     <tableColumn id="14" name=""/>
     <tableColumn id="15" name=""/>
@@ -255,7 +242,6 @@
     <tableColumn id="36" name=""/>
     <tableColumn id="37" name=""/>
     <tableColumn id="38" name=""/>
-    <tableColumn id="39" name=""/>
   </tableColumns>
 </table>
 </file>
@@ -265,23 +251,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="7" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="12.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="2" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -315,9 +301,7 @@
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
@@ -344,48 +328,44 @@
       <c r="AJ1" s="3"/>
       <c r="AK1" s="3"/>
       <c r="AL1" s="3"/>
-      <c r="AM1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
+      <c r="D2" s="5" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="E2" s="6" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="J2" s="7" t="n">
+      <c r="I2" s="6" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K2" s="7" t="n">
+      <c r="J2" s="6" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>15</v>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>